<commit_message>
atualizando ORSD e CQs
</commit_message>
<xml_diff>
--- a/Documentos/Documento de  Especificação de Requisitos da Ontologia - Ontologia das Eleições Brasileiras.xlsx
+++ b/Documentos/Documento de  Especificação de Requisitos da Ontologia - Ontologia das Eleições Brasileiras.xlsx
@@ -5,23 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiqui\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\dissertacao_mestrado\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED3BD9EF-BEFF-4573-9C69-9CF310096BF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFB60DA-EC02-40EF-8A4F-CE5F65EB41E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="v2" sheetId="2" r:id="rId2"/>
+    <sheet name="v2" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="v3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="55">
   <si>
     <t>Documento de  Especificação de Requisitos da Ontologia</t>
   </si>
@@ -45,6 +46,19 @@
   </si>
   <si>
     <t>Usuários</t>
+  </si>
+  <si>
+    <t>Usuário 1 - Pesquisadores e pessoas com interesse no domínio eleitoral brasileiro e desejam fazer uso de recursos ontológicos
+Usuário 2 - Governo brasileiro</t>
+  </si>
+  <si>
+    <t>Usos pretendidos</t>
+  </si>
+  <si>
+    <t>Uso pretendido 1 - Servir como base semântica para o processo de geração de triplas RDF para o domínio das eleições brasileiras</t>
+  </si>
+  <si>
+    <t>Requisitos</t>
   </si>
   <si>
     <r>
@@ -69,19 +83,6 @@
     </r>
   </si>
   <si>
-    <t>Usuário 1 - Pesquisadores e pessoas com interesse no domínio eleitoral brasileiro e desejam fazer uso de recursos ontológicos
-Usuário 2 - Governo brasileiro</t>
-  </si>
-  <si>
-    <t>Usos pretendidos</t>
-  </si>
-  <si>
-    <t>Uso pretendido 1 - Servir como base semântica para o processo de geração de triplas RDF para o domínio das eleições brasileiras</t>
-  </si>
-  <si>
-    <t>Requisitos</t>
-  </si>
-  <si>
     <t>a) Não-funcionais</t>
   </si>
   <si>
@@ -91,54 +92,44 @@
     <t>b) Funcionais</t>
   </si>
   <si>
+    <t>Eleição (7 QCs)</t>
+  </si>
+  <si>
+    <t>Candidato (15 QCs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CQ1 - Em que ano a eleição foi realizada?
+CQ2 - Quais cargos políticos foram disputados na eleição?
+CQ3 - Quem foram os candidatos que disputaram cargos políticos na eleição?
+CQ4 -Quais as zonas eleitorais existentes para a eleição?
+CQ5 - Quais as seções eleitorais existentes para a eleição?
+CQ6 - Qual a porcentagem de participação de eleitores na eleição?
+CQ7 - Qual a porcentagem de abstenção de eleitores na eleição?
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CQ8 - Qual o nome do candidato?
+CQ9 - Qual o partido do candidato?
+CQ10 - Qual a coligação do candidato?
+CQ11 - Qual o número do candidato?
+CQ12 - Qual cargo político o candidato disputou?
+CQ13 - Por qual cidade e/ou estado o candidato disputou a eleição?
+CQ14 - Quantos votos o candidato recebeu?
+CQ15 - O candidato foi eleito?
+CQ16 - O candidato foi caçado?
+CQ17 - Quais os bens declarados pelo candidato?
+CQ18 - Qual o valor de cada bem declarado pelo candidato?
+CQ19 - Quais as fontes de receitas declaradas pelo candidato para sua campanha?
+CQ20 - Quais as fontes de despesas declaradas pelo candidato para sua campanha?
+CQ21 - Qual o valor recebido de cada fonte de receita do candidato em sua campanha?
+CQ22 - Qual o valor gasto em cada fonte de despesa pelo candidato em sua campanha?
+</t>
+  </si>
+  <si>
     <t>Eleição (8 QCs)</t>
   </si>
   <si>
-    <t>Candidato (15 QCs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CQ1 - Em que anos foram realizadas eleições no Brasil?
-CQ2 - Quais cargos políticos são disputados através de eleição no Brasil?
-CQ3 - Quais cargos políticos foram disputados em cada eleição no Brasil?
-CQ4 - Quem foram os candidatos que disputaram cargos políticos nas eleições no Brasil?
-CQ5 - Quais as zonas eleitorais existentes para a eleição?
-CQ6 - Quais as seções eleitorais existentes para a eleição?
-CQ7 - Qual a porcentagem de participação de eleitores na eleição?
-CQ8 - Qual a porcentagem de abstenção de eleitores na eleição?
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CQ9 - Qual o nome do candidato?
-CQ10 - Qual o partido do candidato?
-CQ11 - Qual a coligação do candidato?
-CQ12 - Qual o número do candidato?
-CQ13 - Qual cargo político o candidato disputou?
-CQ14 - Por qual cidade e/ou estado o candidato disputou a eleição?
-CQ15 - Quantos votos o candidato recebeu?
-CQ16 - O candidato foi eleito?
-CQ17 - O candidato foi caçado?
-CQ18 - Quais os bens declarados pelo candidato?
-CQ19 - Qual o valor de cada bem declarado pelo candidato?
-CQ20 - Quais as fontes de receitas declaradas pelo candidato para sua campanha?
-CQ21 - Quais as fontes de despesas declaradas pelo candidato para sua campanha?
-CQ22 - Qual o valor recebido de cada fonte de receita do candidato em sua campanha?
-CQ23 - Qual o valor gasto em cada fonte de despesa pelo candidato em sua campanha?
-</t>
-  </si>
-  <si>
-    <t>Partido (7 QCs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CQ24 - Quais partidos disputaram a eleição?
-CQ25 - Quais coligações foram formadas para disputar a eleição?
-CQ26 - Quais partidos integram cada coligação formada para a eleição?
-</t>
-  </si>
-  <si>
-    <t>Pré-glossário de termos</t>
-  </si>
-  <si>
-    <t>a) Termos das Questões de Competência</t>
+    <t>Partido (3 QCs)</t>
   </si>
   <si>
     <t xml:space="preserve">CQ1 - Em que anos foram realizadas eleições no Brasil?
@@ -150,43 +141,6 @@
 CQ23 - Qual a porcentagem de participação de eleitores na eleição?
 CQ24 - Qual a porcentagem de abstenção de eleitores na eleição?
 </t>
-  </si>
-  <si>
-    <t>eleição - 16
-candidato - 16
-ser - 7
-disputar - 7
-partido - 6
-Brasil - 4
-cargo político - 4
-campanha - 4
-valor - 3
-eleitor - 2
-fonte de receita - 2
-fonte de despesa - 2
-declarar - 2
-receber - 2
-bem - 2
-coligação - 2
-formar - 2</t>
-  </si>
-  <si>
-    <t>porcentagem de participação - 1
-porcentagem de abstenção - 1
-voto - 1
-gastar - 1
-nome - 1
-número - 1
-eleito - 1
-cassado - 1
-ano - 1
-zona eleitoral - 1
-seção eleitoral - 1
-cidade - 1
-estado - 1
-ter - 1
-integrar - 1
-realizar - 1</t>
   </si>
   <si>
     <t>CQ5 - Qual o nome do candidato?
@@ -206,83 +160,19 @@
 CQ19 - Qual o valor gasto em cada fonte de despesa pelo candidato em sua campanha?</t>
   </si>
   <si>
-    <t>b) Termos das respostas</t>
+    <t xml:space="preserve">CQ23 - Quais partidos disputaram a eleição?
+CQ24 - Quais coligações foram formadas para disputar a eleição?
+CQ25 - Quais partidos integram cada coligação formada para a eleição?
+</t>
   </si>
   <si>
     <t>Eleitor (5 QCs)</t>
   </si>
   <si>
-    <t>presidente - 9
-governador - 9
-senador - 9
-deputado federal - 9
-deputado estadual - 9
-vereador - 7
-prefeito - 7
-não informado - 2
-recursos de pessoas físicas - 2
-recursos próprios - 1</t>
-  </si>
-  <si>
-    <t>recursos de partido político - 1
-recursos de outros candidatos - 1
-recursos de Financiamento Coletivo - 1
-recursos de origens não identificadas - 1
-rendimentos de aplicações financeiras - 1
-doações pela Internet - 1
-gênero - 1
-estado cívil - 1
-faixa etária - 1
-grau de escolaridade - 1
-encargos financeiros, taxas bancárias e/ou op. Cartão de crédito - 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diversas a especificar - 1
-publicidade por materiais impressos - 1
-combustíveis e lubrificantes - 1
-despesas com pessoal - 1
-cessão ou locação de veículos - 1
-despesa com impulsionamento de conteúdos - 1
-publicidade por adesivos - 1
-serviços prestados por terceiros - 1
-locação/cessão de bens imóveis - 1
-atividades de militância e mobilização de rua - 1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">publicidade por carros de som - 1
-alimentação - 1
-publicidade por jornais e revistas - 1
-despesas com transporte ou deslocamento - 1
-telefone - 1
-eventos de promoção da candidatura - 1
-taxa de administração de financiamento coletivo - 1
-serviços próprios prestados por terceiros - 1
-locação/cessão de bens móveis (exceto veículos) - 1
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">produção de programas de rádio, televisão ou vídeo - 1
-produção de jingles, vinhetas e slogans - 1
-correspondências e despesas postais - 1
-criação e inclusão de páginas na internet - 1
-doações financeiras a outros candidatos/partidos - 1
-materiais de expediente - 1
-reembolsos de gastos realizados por eleitores - 1
-comícios - 1
-água - 1
-despesas com hospedagem - 1
-</t>
-  </si>
-  <si>
-    <t>impostos, contribuições e taxas - 1
-aquisição/doação de bens móveis ou imóveis - 1
-pré-instalação física de comitê de campanha - 1
-energia elétrica - 1
-passagem aérea - 1
-pesquisas ou testes eleitorais - 1
-encargos sociais - 1
-multas eleitorais - 1</t>
+    <t>Partido (7 QCs)</t>
+  </si>
+  <si>
+    <t>Pré-glossário de termos</t>
   </si>
   <si>
     <r>
@@ -300,9 +190,6 @@
 CQ27 - Qual a porcentagem de votos por faixa etária dos eleitores na eleição?
 CQ28 - Qual a porcentagem de votos por grau de escolaridade dos eleitores na eleição?</t>
     </r>
-  </si>
-  <si>
-    <t>c) Objetos</t>
   </si>
   <si>
     <r>
@@ -324,7 +211,41 @@
     </r>
   </si>
   <si>
-    <t>N/A</t>
+    <t>a) Termos das Questões de Competência</t>
+  </si>
+  <si>
+    <t>candidato - 16
+eleição - 11
+ser - 6
+disputar - 6
+campanha - 4
+eleitor - 4
+declarar - 4
+partido - 3
+cargo político - 3
+valor - 3
+receber - 2
+bem - 2
+coligação - 2
+formar - 2</t>
+  </si>
+  <si>
+    <t>fonte de receita - 1
+fonte de despesa - 1
+porcentagem de participação - 1
+porcentagem de abstenção - 1
+voto - 1
+gastar - 1
+nome - 1
+número - 1
+eleito - 1
+cassado - 1
+ano - 1
+zona eleitoral - 1
+seção eleitoral - 1
+cidade - 1
+estado - 1
+integrar - 1</t>
   </si>
   <si>
     <t>eleição - 16
@@ -372,6 +293,12 @@
 faixa etária - 1
 grau de escolaridade - 1
 integrar - 1</t>
+  </si>
+  <si>
+    <t>b) Termos das respostas</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>presidente - 9
@@ -502,6 +429,25 @@
 seguros - ordinárias - 1</t>
   </si>
   <si>
+    <t>eleição - 16
+candidato - 16
+ser - 7
+disputar - 7
+partido - 6
+Brasil - 4
+cargo político - 4
+campanha - 4
+valor - 3
+eleitor - 2
+fonte de receita - 2
+fonte de despesa - 2
+declarar - 2
+receber - 2
+bem - 2
+coligação - 2
+formar - 2</t>
+  </si>
+  <si>
     <t>rádio e televisão - ordinárias - 1
 pessoal - contribuição sindical - ordinárias - 1
 manutenção, conservação e reparos de bens - ordinárias - 1
@@ -534,6 +480,27 @@
 lanches e refeições - ordinárias - 1</t>
   </si>
   <si>
+    <t>c) Objetos</t>
+  </si>
+  <si>
+    <t>porcentagem de participação - 1
+porcentagem de abstenção - 1
+voto - 1
+gastar - 1
+nome - 1
+número - 1
+eleito - 1
+cassado - 1
+ano - 1
+zona eleitoral - 1
+seção eleitoral - 1
+cidade - 1
+estado - 1
+ter - 1
+integrar - 1
+realizar - 1</t>
+  </si>
+  <si>
     <t>pessoal - alimentação do trabalhador - ordinárias - 1
 pessoal - auxílio-transporte - ordinárias - 1
 pessoal - outras despesas com pessoal - mulheres - 1
@@ -642,6 +609,79 @@
 telecomunicações e internet - mulheres - 1
 pessoal - salários e ordenados - despesas eleitorais - 1
 serviços técnico-profissionais - outros serviços técnicos e profissionais - despesas eleitorais - 1</t>
+  </si>
+  <si>
+    <t>presidente - 9
+governador - 9
+senador - 9
+deputado federal - 9
+deputado estadual - 9
+vereador - 7
+prefeito - 7
+não informado - 2
+recursos de pessoas físicas - 2
+recursos próprios - 1</t>
+  </si>
+  <si>
+    <t>recursos de partido político - 1
+recursos de outros candidatos - 1
+recursos de Financiamento Coletivo - 1
+recursos de origens não identificadas - 1
+rendimentos de aplicações financeiras - 1
+doações pela Internet - 1
+gênero - 1
+estado cívil - 1
+faixa etária - 1
+grau de escolaridade - 1
+encargos financeiros, taxas bancárias e/ou op. Cartão de crédito - 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diversas a especificar - 1
+publicidade por materiais impressos - 1
+combustíveis e lubrificantes - 1
+despesas com pessoal - 1
+cessão ou locação de veículos - 1
+despesa com impulsionamento de conteúdos - 1
+publicidade por adesivos - 1
+serviços prestados por terceiros - 1
+locação/cessão de bens imóveis - 1
+atividades de militância e mobilização de rua - 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publicidade por carros de som - 1
+alimentação - 1
+publicidade por jornais e revistas - 1
+despesas com transporte ou deslocamento - 1
+telefone - 1
+eventos de promoção da candidatura - 1
+taxa de administração de financiamento coletivo - 1
+serviços próprios prestados por terceiros - 1
+locação/cessão de bens móveis (exceto veículos) - 1
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">produção de programas de rádio, televisão ou vídeo - 1
+produção de jingles, vinhetas e slogans - 1
+correspondências e despesas postais - 1
+criação e inclusão de páginas na internet - 1
+doações financeiras a outros candidatos/partidos - 1
+materiais de expediente - 1
+reembolsos de gastos realizados por eleitores - 1
+comícios - 1
+água - 1
+despesas com hospedagem - 1
+</t>
+  </si>
+  <si>
+    <t>impostos, contribuições e taxas - 1
+aquisição/doação de bens móveis ou imóveis - 1
+pré-instalação física de comitê de campanha - 1
+energia elétrica - 1
+passagem aérea - 1
+pesquisas ou testes eleitorais - 1
+encargos sociais - 1
+multas eleitorais - 1</t>
   </si>
 </sst>
 </file>
@@ -1131,9 +1171,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1181,7 +1219,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="1"/>
       <c r="F3" s="15" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="1"/>
@@ -1261,7 +1299,7 @@
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
@@ -1276,7 +1314,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
@@ -1289,7 +1327,7 @@
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
@@ -1304,7 +1342,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
@@ -1356,7 +1394,7 @@
     <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>17</v>
@@ -1371,10 +1409,10 @@
     <row r="17" spans="1:10" ht="178.5" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="1"/>
@@ -1386,10 +1424,10 @@
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="1"/>
@@ -1401,10 +1439,10 @@
     <row r="19" spans="1:10" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="1"/>
@@ -1418,7 +1456,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="12"/>
@@ -1431,7 +1469,7 @@
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="13" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
@@ -1444,10 +1482,10 @@
     <row r="22" spans="1:10" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="5" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="1"/>
@@ -1459,7 +1497,7 @@
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="13" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="12"/>
@@ -1472,25 +1510,25 @@
     <row r="24" spans="1:10" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1502,13 +1540,13 @@
     <row r="26" spans="1:10" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1520,7 +1558,7 @@
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="13" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="12"/>
@@ -1533,7 +1571,7 @@
     <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="3"/>
       <c r="B28" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="12"/>
@@ -1583,9 +1621,7 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1711,7 +1747,7 @@
     <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="12"/>
@@ -1726,7 +1762,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="11"/>
       <c r="D10" s="12"/>
@@ -1739,7 +1775,7 @@
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12"/>
@@ -1754,7 +1790,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12"/>
@@ -1818,7 +1854,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="178.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="5" t="s">
         <v>18</v>
@@ -1836,7 +1872,7 @@
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="12"/>
@@ -1849,7 +1885,7 @@
     <row r="19" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="5" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="12"/>
@@ -1864,7 +1900,7 @@
         <v>7</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="12"/>
@@ -1877,7 +1913,7 @@
     <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="13" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12"/>
@@ -1890,10 +1926,10 @@
     <row r="22" spans="1:10" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="1"/>
@@ -1905,7 +1941,7 @@
     <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="3"/>
       <c r="B23" s="13" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="12"/>
@@ -1918,25 +1954,25 @@
     <row r="24" spans="1:10" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="5" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="5" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1948,7 +1984,7 @@
     <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="3"/>
       <c r="B26" s="13" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="12"/>
@@ -1961,7 +1997,7 @@
     <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="3"/>
       <c r="B27" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="12"/>
@@ -2001,4 +2037,416 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" customWidth="1"/>
+    <col min="5" max="9" width="43.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>6</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="12"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="17"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>7</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="1:10" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="26">
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>